<commit_message>
Se corrigen las validaciones
</commit_message>
<xml_diff>
--- a/outputs/validacion/auditoria_validacion.xlsx
+++ b/outputs/validacion/auditoria_validacion.xlsx
@@ -545,13 +545,13 @@
         <v>500</v>
       </c>
       <c r="F2">
-        <v>0.003741300000000006</v>
+        <v>0.003735560000000006</v>
       </c>
       <c r="G2">
-        <v>0.005005785912321867</v>
+        <v>0.005003107714211245</v>
       </c>
       <c r="H2">
-        <v>0.3393528118655694</v>
+        <v>0.3388102804134973</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -563,13 +563,13 @@
         <v>500</v>
       </c>
       <c r="L2">
-        <v>0.003741300000000006</v>
+        <v>0.003735560000000006</v>
       </c>
       <c r="M2">
-        <v>0.005005785912321867</v>
+        <v>0.005003107714211245</v>
       </c>
       <c r="N2">
-        <v>0.3393528118655694</v>
+        <v>0.3388102804134973</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -589,13 +589,13 @@
         <v>500</v>
       </c>
       <c r="F3">
-        <v>0.004500917335128795</v>
+        <v>0.004470761978683473</v>
       </c>
       <c r="G3">
-        <v>0.006081953699466782</v>
+        <v>0.006090099392694067</v>
       </c>
       <c r="H3">
-        <v>0.4082477348662198</v>
+        <v>0.4055358688775248</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -607,13 +607,13 @@
         <v>500</v>
       </c>
       <c r="L3">
-        <v>0.004500917335128795</v>
+        <v>0.004470761978683473</v>
       </c>
       <c r="M3">
-        <v>0.006081953699466782</v>
+        <v>0.006090099392694067</v>
       </c>
       <c r="N3">
-        <v>0.4082477348662198</v>
+        <v>0.4055358688775248</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -633,13 +633,13 @@
         <v>500</v>
       </c>
       <c r="F4">
-        <v>0.01579720738959127</v>
+        <v>0.01580027341018982</v>
       </c>
       <c r="G4">
-        <v>0.02100213740777539</v>
+        <v>0.02099419234259793</v>
       </c>
       <c r="H4">
-        <v>1.436187325315414</v>
+        <v>1.43649118887672</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -651,13 +651,13 @@
         <v>500</v>
       </c>
       <c r="L4">
-        <v>0.01579720738959127</v>
+        <v>0.01580027341018982</v>
       </c>
       <c r="M4">
-        <v>0.02100213740777539</v>
+        <v>0.02099419234259793</v>
       </c>
       <c r="N4">
-        <v>1.436187325315414</v>
+        <v>1.43649118887672</v>
       </c>
     </row>
   </sheetData>
@@ -701,6 +701,15 @@
         <v>25</v>
       </c>
       <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
@@ -712,7 +721,16 @@
         <v>26</v>
       </c>
       <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>48.6</v>
+      </c>
+      <c r="E3">
         <v>0</v>
+      </c>
+      <c r="F3">
+        <v>51.4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -726,13 +744,13 @@
         <v>500</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>39.2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>22.4</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -743,7 +761,16 @@
         <v>25</v>
       </c>
       <c r="C5">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <v>47.59999999999999</v>
+      </c>
+      <c r="E5">
         <v>0</v>
+      </c>
+      <c r="F5">
+        <v>52.40000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -754,7 +781,16 @@
         <v>26</v>
       </c>
       <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6">
+        <v>48.6</v>
+      </c>
+      <c r="E6">
         <v>0</v>
+      </c>
+      <c r="F6">
+        <v>51.4</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -768,13 +804,13 @@
         <v>500</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>29.6</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>37.4</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -785,7 +821,16 @@
         <v>25</v>
       </c>
       <c r="C8">
+        <v>500</v>
+      </c>
+      <c r="D8">
+        <v>37.6</v>
+      </c>
+      <c r="E8">
         <v>0</v>
+      </c>
+      <c r="F8">
+        <v>62.4</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -796,7 +841,16 @@
         <v>26</v>
       </c>
       <c r="C9">
+        <v>500</v>
+      </c>
+      <c r="D9">
+        <v>48.6</v>
+      </c>
+      <c r="E9">
         <v>0</v>
+      </c>
+      <c r="F9">
+        <v>51.4</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -810,13 +864,13 @@
         <v>500</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>34.59999999999999</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>60.2</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +908,7 @@
         <v>33</v>
       </c>
       <c r="C2">
-        <v>3.614935514975448E-16</v>
+        <v>1.61394316183885E-16</v>
       </c>
       <c r="D2">
         <v>0.9999999999999998</v>
@@ -882,10 +936,10 @@
         <v>34</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-1.670833306185265E-15</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.9999999999999987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>